<commit_message>
working through trait measurements
</commit_message>
<xml_diff>
--- a/raw data/Slide_ID.xlsx
+++ b/raw data/Slide_ID.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\Projects\ant_habitat_coexistence\raw data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598D187A-8E71-430C-9A29-AA434B883205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91150F3-EDD3-4F42-948C-1AC4E5FE7302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H273"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A272" sqref="A272"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="E141" sqref="E141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3106,7 +3106,7 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B138" t="s">
         <v>46</v>
@@ -3126,7 +3126,7 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B139" t="s">
         <v>46</v>
@@ -3146,7 +3146,7 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B140" t="s">
         <v>46</v>
@@ -3166,7 +3166,7 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B141" t="s">
         <v>46</v>
@@ -3186,7 +3186,7 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B142" t="s">
         <v>46</v>
@@ -3206,7 +3206,7 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B143" t="s">
         <v>46</v>
@@ -3226,7 +3226,7 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B144" t="s">
         <v>78</v>
@@ -3246,7 +3246,7 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B145" t="s">
         <v>78</v>
@@ -3266,7 +3266,7 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B146" t="s">
         <v>78</v>
@@ -3286,7 +3286,7 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B147" t="s">
         <v>78</v>
@@ -3306,7 +3306,7 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B148" t="s">
         <v>78</v>
@@ -3326,7 +3326,7 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B149" t="s">
         <v>78</v>
@@ -8698,7 +8698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>